<commit_message>
added HR course material
</commit_message>
<xml_diff>
--- a/Python ETL/BASE_DADOS-ELETRONICA-1.1.xlsx
+++ b/Python ETL/BASE_DADOS-ELETRONICA-1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolineamarante/Documents/gerenciamento-de-salas-V0.1/Python ETL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11800393-048E-E141-BE54-A81E8767D51C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61513FF3-209D-AC4C-9509-392617B400BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14900" activeTab="6" xr2:uid="{DE615C08-F97B-4A36-9702-3D0A64471026}"/>
   </bookViews>
@@ -2715,7 +2715,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.1640625" defaultRowHeight="15"/>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="D1" s="31">
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E1" s="142" t="s">
         <v>162</v>
@@ -2853,21 +2853,21 @@
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>134</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>137</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="J4" s="24" t="s">
         <v>140</v>
@@ -2928,35 +2928,35 @@
       <c r="B6" s="135"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>131</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>134</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>72</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="J6" s="24" t="s">
         <v>140</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="L6" s="24" t="s">
         <v>128</v>
@@ -3026,7 +3026,7 @@
       <c r="B9" s="135"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>131</v>
@@ -3047,14 +3047,14 @@
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>140</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="L9" s="24" t="s">
         <v>128</v>
@@ -3108,35 +3108,35 @@
       <c r="B11" s="135"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>131</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>134</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>137</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="J11" s="24" t="s">
         <v>140</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="L11" s="24" t="s">
         <v>128</v>
@@ -3190,21 +3190,21 @@
       <c r="B13" s="137"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>131</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>134</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="H13" s="27" t="s">
         <v>72</v>
@@ -3218,7 +3218,7 @@
       </c>
       <c r="K13" s="47">
         <f>VLOOKUP(L13,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="L13" s="24" t="s">
         <v>128</v>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="D1" s="31">
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E1" s="142" t="s">
         <v>163</v>
@@ -3415,35 +3415,35 @@
       <c r="B4" s="135"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>137</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>128</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>128</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="J4" s="24" t="s">
         <v>71</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="L4" s="25" t="s">
         <v>128</v>
@@ -3497,28 +3497,28 @@
       <c r="B6" s="135"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>137</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>128</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>128</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="J6" s="24" t="s">
         <v>71</v>
@@ -3595,35 +3595,35 @@
       <c r="B9" s="135"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>140</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>134</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>128</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>71</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="L9" s="25" t="s">
         <v>134</v>
@@ -3677,35 +3677,35 @@
       <c r="B11" s="135"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>140</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>137</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>128</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="J11" s="24" t="s">
         <v>71</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="L11" s="25" t="s">
         <v>134</v>
@@ -3759,35 +3759,35 @@
       <c r="B13" s="137"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>140</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>137</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>128</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="J13" s="27" t="s">
         <v>140</v>
       </c>
       <c r="K13" s="23">
         <f>VLOOKUP(L13,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="L13" s="25" t="s">
         <v>134</v>
@@ -3870,7 +3870,7 @@
       </c>
       <c r="D1" s="31">
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E1" s="142" t="s">
         <v>164</v>
@@ -3970,35 +3970,35 @@
       <c r="B4" s="135"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>128</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>146</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>146</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="J4" s="24" t="s">
         <v>128</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="L4" s="25" t="s">
         <v>134</v>
@@ -4052,35 +4052,35 @@
       <c r="B6" s="135"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>143</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>146</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>147</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="J6" s="24" t="s">
         <v>128</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>134</v>
@@ -4150,35 +4150,35 @@
       <c r="B9" s="135"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>143</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>146</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>147</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>128</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="L9" s="25" t="s">
         <v>151</v>
@@ -4232,35 +4232,35 @@
       <c r="B11" s="135"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>143</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>128</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>147</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="J11" s="24" t="s">
         <v>128</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="L11" s="25" t="s">
         <v>151</v>
@@ -4314,28 +4314,28 @@
       <c r="B13" s="137"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>143</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>128</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>147</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="J13" s="24" t="s">
         <v>128</v>
@@ -4431,7 +4431,7 @@
       </c>
       <c r="D1" s="20">
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E1" s="142" t="s">
         <v>165</v>
@@ -4531,21 +4531,21 @@
       <c r="B4" s="135"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>131</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>131</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>131</v>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="L4" s="25" t="s">
         <v>156</v>
@@ -4613,35 +4613,35 @@
       <c r="B6" s="135"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>128</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>131</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>131</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="J6" s="24" t="s">
         <v>143</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>156</v>
@@ -4711,35 +4711,35 @@
       <c r="B9" s="135"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>128</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>131</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>131</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>143</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="L9" s="25" t="s">
         <v>156</v>
@@ -4793,35 +4793,35 @@
       <c r="B11" s="135"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>128</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>72</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>153</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="J11" s="24" t="s">
         <v>143</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="L11" s="25" t="s">
         <v>156</v>
@@ -4875,35 +4875,35 @@
       <c r="B13" s="137"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>128</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>72</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>153</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="J13" s="24" t="s">
         <v>143</v>
       </c>
       <c r="K13" s="23">
         <f>VLOOKUP(L13,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="L13" s="25" t="s">
         <v>131</v>
@@ -4985,7 +4985,7 @@
       </c>
       <c r="D1" s="31">
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E1" s="142" t="s">
         <v>166</v>
@@ -5085,35 +5085,35 @@
       <c r="B4" s="135"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>143</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>159</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>71</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="J4" s="24" t="s">
         <v>131</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="L4" s="25" t="s">
         <v>143</v>
@@ -5167,35 +5167,35 @@
       <c r="B6" s="135"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>84</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>159</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>71</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="J6" s="24" t="s">
         <v>131</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>143</v>
@@ -5265,35 +5265,35 @@
       <c r="B9" s="135"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>84</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>143</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>71</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>131</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="L9" s="25" t="s">
         <v>143</v>
@@ -5347,35 +5347,35 @@
       <c r="B11" s="135"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>70</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>143</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>71</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="J11" s="24" t="s">
         <v>131</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="L11" s="25" t="s">
         <v>143</v>
@@ -5429,28 +5429,28 @@
       <c r="B13" s="137"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>70</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>131</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H13" s="27" t="s">
         <v>143</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="J13" s="24" t="s">
         <v>131</v>
@@ -5538,7 +5538,7 @@
       </c>
       <c r="D1" s="31">
         <f>VLOOKUP(E1,Tabela36[#All],2,FALSE)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E1" s="142" t="s">
         <v>167</v>
@@ -5638,35 +5638,35 @@
       <c r="B4" s="135"/>
       <c r="C4" s="2">
         <f>VLOOKUP(D4,Tabela3[#All],2,FALSE)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>159</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>72</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>143</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="J4" s="24" t="s">
         <v>143</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="L4" s="25" t="s">
         <v>131</v>
@@ -5720,35 +5720,35 @@
       <c r="B6" s="135"/>
       <c r="C6" s="2">
         <f>VLOOKUP(D6,Tabela3[#All],2,FALSE)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>159</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>72</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>143</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="J6" s="24" t="s">
         <v>146</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="L6" s="25" t="s">
         <v>131</v>
@@ -5818,35 +5818,35 @@
       <c r="B9" s="135"/>
       <c r="C9" s="2">
         <f>VLOOKUP(D9,Tabela3[#All],2,FALSE)</f>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>70</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>159</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H9" s="24" t="s">
         <v>143</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>146</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="L9" s="25" t="s">
         <v>131</v>
@@ -5900,35 +5900,35 @@
       <c r="B11" s="135"/>
       <c r="C11" s="2">
         <f>VLOOKUP(D11,Tabela3[#All],2,FALSE)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>159</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>159</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>131</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="J11" s="24" t="s">
         <v>146</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="L11" s="25" t="s">
         <v>131</v>
@@ -5982,28 +5982,28 @@
       <c r="B13" s="137"/>
       <c r="C13" s="23">
         <f>VLOOKUP(D13,Tabela3[#All],2,FALSE)</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>159</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>70</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>131</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="J13" s="24" t="s">
         <v>146</v>
@@ -6075,8 +6075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF6508E-B8F4-43C4-AACB-99409B526617}">
   <dimension ref="B1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -6225,7 +6225,7 @@
         <v>162</v>
       </c>
       <c r="Q4" s="17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S4" s="40" t="s">
         <v>26</v>
@@ -6277,7 +6277,7 @@
         <v>163</v>
       </c>
       <c r="Q5" s="17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="S5" s="40" t="s">
         <v>28</v>
@@ -6299,8 +6299,7 @@
         <v>72</v>
       </c>
       <c r="F6" s="15">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>69</v>
@@ -6329,7 +6328,7 @@
         <v>164</v>
       </c>
       <c r="Q6" s="17">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="S6" s="40" t="s">
         <v>30</v>
@@ -6351,8 +6350,7 @@
         <v>128</v>
       </c>
       <c r="F7" s="15">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>129</v>
@@ -6381,7 +6379,7 @@
         <v>165</v>
       </c>
       <c r="Q7" s="17">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="S7" s="40" t="s">
         <v>32</v>
@@ -6403,8 +6401,7 @@
         <v>131</v>
       </c>
       <c r="F8" s="15">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>132</v>
@@ -6433,7 +6430,7 @@
         <v>166</v>
       </c>
       <c r="Q8" s="17">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="S8" s="42" t="s">
         <v>33</v>
@@ -6455,8 +6452,7 @@
         <v>134</v>
       </c>
       <c r="F9" s="15">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>135</v>
@@ -6484,8 +6480,8 @@
       <c r="P9" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="Q9" s="18">
-        <v>6</v>
+      <c r="Q9" s="17">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:20">
@@ -6501,8 +6497,7 @@
         <v>137</v>
       </c>
       <c r="F10" s="15">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>138</v>
@@ -6542,8 +6537,7 @@
         <v>140</v>
       </c>
       <c r="F11" s="15">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>141</v>
@@ -6583,8 +6577,7 @@
         <v>71</v>
       </c>
       <c r="F12" s="15">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>6</v>
@@ -6624,8 +6617,7 @@
         <v>143</v>
       </c>
       <c r="F13" s="15">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>144</v>
@@ -6665,8 +6657,7 @@
         <v>146</v>
       </c>
       <c r="F14" s="15">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>65</v>
@@ -6706,8 +6697,7 @@
         <v>147</v>
       </c>
       <c r="F15" s="15">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>65</v>
@@ -6747,8 +6737,7 @@
         <v>151</v>
       </c>
       <c r="F16" s="15">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>152</v>
@@ -6788,8 +6777,7 @@
         <v>153</v>
       </c>
       <c r="F17" s="15">
-        <f t="shared" si="1"/>
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>154</v>
@@ -6829,8 +6817,7 @@
         <v>156</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>65</v>
@@ -6870,8 +6857,7 @@
         <v>84</v>
       </c>
       <c r="F19" s="15">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>65</v>
@@ -6911,8 +6897,7 @@
         <v>70</v>
       </c>
       <c r="F20" s="15">
-        <f>ROW() - 3</f>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>158</v>
@@ -6952,8 +6937,7 @@
         <v>159</v>
       </c>
       <c r="F21" s="15">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>160</v>
@@ -6990,15 +6974,10 @@
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="80"/>
-      <c r="F22" s="15">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
+      <c r="F22" s="15"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="13">
-        <v>5</v>
-      </c>
+      <c r="I22" s="13"/>
       <c r="J22" s="12"/>
       <c r="K22" s="83" t="s">
         <v>15</v>
@@ -7025,14 +7004,9 @@
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="80"/>
-      <c r="F23" s="15">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
+      <c r="F23" s="15"/>
       <c r="H23" s="130"/>
-      <c r="I23" s="13">
-        <v>7</v>
-      </c>
+      <c r="I23" s="13"/>
       <c r="J23" s="12"/>
       <c r="K23" s="83" t="s">
         <v>42</v>
@@ -7685,7 +7659,7 @@
       </c>
       <c r="H3" s="105">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I3" s="105">
         <f>'1_SEMESTRE'!A2</f>
@@ -7716,7 +7690,7 @@
       </c>
       <c r="F4" s="15">
         <f>'1_SEMESTRE'!C6</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G4" s="98">
         <f>'1_SEMESTRE'!C5</f>
@@ -7724,7 +7698,7 @@
       </c>
       <c r="H4" s="99">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I4" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -7755,7 +7729,7 @@
       </c>
       <c r="F5" s="15">
         <f>'1_SEMESTRE'!C9</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G5" s="98">
         <f>'1_SEMESTRE'!C8</f>
@@ -7763,7 +7737,7 @@
       </c>
       <c r="H5" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I5" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -7794,7 +7768,7 @@
       </c>
       <c r="F6" s="15">
         <f>'1_SEMESTRE'!C11</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G6" s="98">
         <f>'1_SEMESTRE'!C10</f>
@@ -7802,7 +7776,7 @@
       </c>
       <c r="H6" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I6" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -7834,7 +7808,7 @@
       </c>
       <c r="F7" s="15">
         <f>'1_SEMESTRE'!C13</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G7" s="98">
         <f>'1_SEMESTRE'!C12</f>
@@ -7842,7 +7816,7 @@
       </c>
       <c r="H7" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I7" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -7874,7 +7848,7 @@
       </c>
       <c r="F8" s="15">
         <f>'1_SEMESTRE'!E4</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G8" s="98">
         <f>'1_SEMESTRE'!E3</f>
@@ -7882,7 +7856,7 @@
       </c>
       <c r="H8" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I8" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -7914,7 +7888,7 @@
       </c>
       <c r="F9" s="15">
         <f>'1_SEMESTRE'!E4</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G9" s="98">
         <f>'1_SEMESTRE'!E5</f>
@@ -7922,7 +7896,7 @@
       </c>
       <c r="H9" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I9" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -7962,7 +7936,7 @@
       </c>
       <c r="H10" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I10" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -7994,7 +7968,7 @@
       </c>
       <c r="F11" s="15">
         <f>'1_SEMESTRE'!E11</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G11" s="98">
         <f>'1_SEMESTRE'!E10</f>
@@ -8002,7 +7976,7 @@
       </c>
       <c r="H11" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I11" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8034,7 +8008,7 @@
       </c>
       <c r="F12" s="15">
         <f>'1_SEMESTRE'!E13</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G12" s="98">
         <f>'1_SEMESTRE'!E12</f>
@@ -8042,7 +8016,7 @@
       </c>
       <c r="H12" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I12" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8074,7 +8048,7 @@
       </c>
       <c r="F13" s="15">
         <f>'1_SEMESTRE'!G4</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G13" s="98">
         <f>'1_SEMESTRE'!G3</f>
@@ -8082,7 +8056,7 @@
       </c>
       <c r="H13" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I13" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8114,7 +8088,7 @@
       </c>
       <c r="F14" s="15">
         <f>'1_SEMESTRE'!G6</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G14" s="98">
         <f>'1_SEMESTRE'!G5</f>
@@ -8122,7 +8096,7 @@
       </c>
       <c r="H14" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I14" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8162,7 +8136,7 @@
       </c>
       <c r="H15" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I15" s="99">
         <f>'1_SEMESTRE'!A2</f>
@@ -8194,7 +8168,7 @@
       </c>
       <c r="F16" s="15">
         <f>'1_SEMESTRE'!G11</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G16" s="98">
         <f>'1_SEMESTRE'!G10</f>
@@ -8202,7 +8176,7 @@
       </c>
       <c r="H16" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I16" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8234,7 +8208,7 @@
       </c>
       <c r="F17" s="15">
         <f>'1_SEMESTRE'!G13</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G17" s="98">
         <f>'1_SEMESTRE'!G12</f>
@@ -8242,7 +8216,7 @@
       </c>
       <c r="H17" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I17" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8274,7 +8248,7 @@
       </c>
       <c r="F18" s="15">
         <f>'1_SEMESTRE'!I4</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G18" s="15">
         <f>'1_SEMESTRE'!I3</f>
@@ -8282,7 +8256,7 @@
       </c>
       <c r="H18" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I18" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8314,7 +8288,7 @@
       </c>
       <c r="F19" s="15">
         <f>'1_SEMESTRE'!I6</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G19" s="15">
         <f>'1_SEMESTRE'!I5</f>
@@ -8322,7 +8296,7 @@
       </c>
       <c r="H19" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I19" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8354,7 +8328,7 @@
       </c>
       <c r="F20" s="15">
         <f>'1_SEMESTRE'!I9</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G20" s="15">
         <f>'1_SEMESTRE'!I8</f>
@@ -8362,7 +8336,7 @@
       </c>
       <c r="H20" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I20" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8394,7 +8368,7 @@
       </c>
       <c r="F21" s="15">
         <f>'1_SEMESTRE'!I11</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G21" s="15">
         <f>'1_SEMESTRE'!I10</f>
@@ -8402,7 +8376,7 @@
       </c>
       <c r="H21" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I21" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8442,7 +8416,7 @@
       </c>
       <c r="H22" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I22" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8482,7 +8456,7 @@
       </c>
       <c r="H23" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I23" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8514,7 +8488,7 @@
       </c>
       <c r="F24" s="15">
         <f>'1_SEMESTRE'!K6</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G24" s="98">
         <f>'1_SEMESTRE'!K5</f>
@@ -8522,7 +8496,7 @@
       </c>
       <c r="H24" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I24" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8554,7 +8528,7 @@
       </c>
       <c r="F25" s="15">
         <f>'1_SEMESTRE'!K9</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G25" s="98">
         <f>'1_SEMESTRE'!K8</f>
@@ -8562,7 +8536,7 @@
       </c>
       <c r="H25" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I25" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8594,7 +8568,7 @@
       </c>
       <c r="F26" s="15">
         <f>'1_SEMESTRE'!K11</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G26" s="98">
         <f>'1_SEMESTRE'!K10</f>
@@ -8602,7 +8576,7 @@
       </c>
       <c r="H26" s="15">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I26" s="15">
         <f>'1_SEMESTRE'!A2</f>
@@ -8634,7 +8608,7 @@
       </c>
       <c r="F27" s="81">
         <f>'1_SEMESTRE'!K13</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G27" s="117">
         <f>'1_SEMESTRE'!K12</f>
@@ -8642,7 +8616,7 @@
       </c>
       <c r="H27" s="81">
         <f>'1_SEMESTRE'!D1</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I27" s="81">
         <f>'1_SEMESTRE'!A2</f>
@@ -8674,7 +8648,7 @@
       </c>
       <c r="F28" s="105">
         <f>'2_SEMESTRE'!C4</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G28" s="118">
         <f>'2_SEMESTRE'!C3</f>
@@ -8682,7 +8656,7 @@
       </c>
       <c r="H28" s="104">
         <f>'2_SEMESTRE'!D1</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I28" s="105">
         <f>'2_SEMESTRE'!A2</f>
@@ -8714,7 +8688,7 @@
       </c>
       <c r="F29" s="15">
         <f>'2_SEMESTRE'!C6</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G29" s="119">
         <f>'2_SEMESTRE'!C5</f>
@@ -8753,7 +8727,7 @@
       </c>
       <c r="F30" s="15">
         <f>'2_SEMESTRE'!C9</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G30" s="119">
         <f>'2_SEMESTRE'!C8</f>
@@ -8792,7 +8766,7 @@
       </c>
       <c r="F31" s="15">
         <f>'2_SEMESTRE'!C11</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G31" s="119">
         <f>'2_SEMESTRE'!C10</f>
@@ -8831,7 +8805,7 @@
       </c>
       <c r="F32" s="15">
         <f>'2_SEMESTRE'!C13</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G32" s="119">
         <f>'2_SEMESTRE'!C12</f>
@@ -8870,7 +8844,7 @@
       </c>
       <c r="F33" s="15">
         <f>'2_SEMESTRE'!E4</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G33" s="44">
         <f>'2_SEMESTRE'!E3</f>
@@ -8909,7 +8883,7 @@
       </c>
       <c r="F34" s="15">
         <f>'2_SEMESTRE'!E6</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G34" s="44">
         <f>'2_SEMESTRE'!E5</f>
@@ -8948,7 +8922,7 @@
       </c>
       <c r="F35" s="15">
         <f>'2_SEMESTRE'!E9</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G35" s="44">
         <f>'2_SEMESTRE'!E8</f>
@@ -8987,7 +8961,7 @@
       </c>
       <c r="F36" s="15">
         <f>'2_SEMESTRE'!E11</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G36" s="44">
         <f>'2_SEMESTRE'!E10</f>
@@ -9026,7 +9000,7 @@
       </c>
       <c r="F37" s="15">
         <f>'2_SEMESTRE'!E13</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G37" s="44">
         <f>'2_SEMESTRE'!E12</f>
@@ -9065,7 +9039,7 @@
       </c>
       <c r="F38" s="15">
         <f>'2_SEMESTRE'!G4</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G38" s="44">
         <f>'2_SEMESTRE'!G3</f>
@@ -9104,7 +9078,7 @@
       </c>
       <c r="F39" s="15">
         <f>'2_SEMESTRE'!G6</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G39" s="44">
         <f>'2_SEMESTRE'!G5</f>
@@ -9143,7 +9117,7 @@
       </c>
       <c r="F40" s="15">
         <f>'2_SEMESTRE'!G9</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G40" s="44">
         <f>'2_SEMESTRE'!G8</f>
@@ -9182,7 +9156,7 @@
       </c>
       <c r="F41" s="15">
         <f>'2_SEMESTRE'!G11</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G41" s="44">
         <f>'2_SEMESTRE'!G10</f>
@@ -9221,7 +9195,7 @@
       </c>
       <c r="F42" s="15">
         <f>'2_SEMESTRE'!G13</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G42" s="44">
         <f>'2_SEMESTRE'!G12</f>
@@ -9260,7 +9234,7 @@
       </c>
       <c r="F43" s="15">
         <f>'2_SEMESTRE'!I4</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G43" s="44">
         <f>'2_SEMESTRE'!I3</f>
@@ -9299,7 +9273,7 @@
       </c>
       <c r="F44" s="15">
         <f>'2_SEMESTRE'!I6</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G44" s="44">
         <f>'2_SEMESTRE'!I5</f>
@@ -9338,7 +9312,7 @@
       </c>
       <c r="F45" s="15">
         <f>'2_SEMESTRE'!I9</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G45" s="44">
         <f>'2_SEMESTRE'!I8</f>
@@ -9377,7 +9351,7 @@
       </c>
       <c r="F46" s="15">
         <f>'2_SEMESTRE'!I11</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G46" s="44">
         <f>'2_SEMESTRE'!I10</f>
@@ -9416,7 +9390,7 @@
       </c>
       <c r="F47" s="15">
         <f>'2_SEMESTRE'!I13</f>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G47" s="44">
         <f>'2_SEMESTRE'!I12</f>
@@ -9455,7 +9429,7 @@
       </c>
       <c r="F48" s="15">
         <f>'2_SEMESTRE'!K4</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G48" s="44">
         <f>'2_SEMESTRE'!K3</f>
@@ -9533,7 +9507,7 @@
       </c>
       <c r="F50" s="15">
         <f>'2_SEMESTRE'!K9</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G50" s="44">
         <f>'2_SEMESTRE'!K8</f>
@@ -9572,7 +9546,7 @@
       </c>
       <c r="F51" s="15">
         <f>'2_SEMESTRE'!K11</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G51" s="44">
         <f>'2_SEMESTRE'!K10</f>
@@ -9611,7 +9585,7 @@
       </c>
       <c r="F52" s="81">
         <f>'2_SEMESTRE'!K13</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G52" s="116">
         <f>'2_SEMESTRE'!K12</f>
@@ -9650,7 +9624,7 @@
       </c>
       <c r="F53" s="105">
         <f>'3_SEMESTRE'!C4</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G53" s="104">
         <f>'3_SEMESTRE'!C3</f>
@@ -9689,7 +9663,7 @@
       </c>
       <c r="F54" s="15">
         <f>'3_SEMESTRE'!C6</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G54" s="44">
         <f>'3_SEMESTRE'!C5</f>
@@ -9728,7 +9702,7 @@
       </c>
       <c r="F55" s="15">
         <f>'3_SEMESTRE'!C9</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G55" s="44">
         <f>'3_SEMESTRE'!C8</f>
@@ -9767,7 +9741,7 @@
       </c>
       <c r="F56" s="15">
         <f>'3_SEMESTRE'!C11</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G56" s="44">
         <f>'3_SEMESTRE'!C10</f>
@@ -9806,7 +9780,7 @@
       </c>
       <c r="F57" s="15">
         <f>'3_SEMESTRE'!C13</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G57" s="44">
         <f>'3_SEMESTRE'!C12</f>
@@ -9845,7 +9819,7 @@
       </c>
       <c r="F58" s="15">
         <f>'3_SEMESTRE'!E4</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G58" s="44">
         <f>'3_SEMESTRE'!E3</f>
@@ -9884,7 +9858,7 @@
       </c>
       <c r="F59" s="15">
         <f>'3_SEMESTRE'!E6</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G59" s="44">
         <f>'3_SEMESTRE'!E5</f>
@@ -9923,7 +9897,7 @@
       </c>
       <c r="F60" s="15">
         <f>'3_SEMESTRE'!E9</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G60" s="44">
         <f>'3_SEMESTRE'!E8</f>
@@ -9962,7 +9936,7 @@
       </c>
       <c r="F61" s="15">
         <f>'3_SEMESTRE'!E11</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G61" s="44">
         <f>'3_SEMESTRE'!E10</f>
@@ -10001,7 +9975,7 @@
       </c>
       <c r="F62" s="15">
         <f>'3_SEMESTRE'!E13</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G62" s="44">
         <f>'3_SEMESTRE'!E12</f>
@@ -10040,7 +10014,7 @@
       </c>
       <c r="F63" s="15">
         <f>'3_SEMESTRE'!G4</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G63" s="44">
         <f>'3_SEMESTRE'!G3</f>
@@ -10079,7 +10053,7 @@
       </c>
       <c r="F64" s="15">
         <f>'3_SEMESTRE'!G6</f>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G64" s="44">
         <f>'3_SEMESTRE'!G5</f>
@@ -10118,7 +10092,7 @@
       </c>
       <c r="F65" s="15">
         <f>'3_SEMESTRE'!G9</f>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G65" s="44">
         <f>'3_SEMESTRE'!G8</f>
@@ -10157,7 +10131,7 @@
       </c>
       <c r="F66" s="15">
         <f>'3_SEMESTRE'!G11</f>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G66" s="44">
         <f>'3_SEMESTRE'!G10</f>
@@ -10196,7 +10170,7 @@
       </c>
       <c r="F67" s="15">
         <f>'3_SEMESTRE'!G13</f>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G67" s="44">
         <f>'3_SEMESTRE'!G12</f>
@@ -10235,7 +10209,7 @@
       </c>
       <c r="F68" s="15">
         <f>'3_SEMESTRE'!I4</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G68" s="44">
         <f>'3_SEMESTRE'!I3</f>
@@ -10274,7 +10248,7 @@
       </c>
       <c r="F69" s="15">
         <f>'3_SEMESTRE'!I6</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G69" s="44">
         <v>5</v>
@@ -10312,7 +10286,7 @@
       </c>
       <c r="F70" s="15">
         <f>'3_SEMESTRE'!I9</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G70" s="44">
         <v>8</v>
@@ -10350,7 +10324,7 @@
       </c>
       <c r="F71" s="15">
         <f>'3_SEMESTRE'!I11</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G71" s="44">
         <v>10</v>
@@ -10388,7 +10362,7 @@
       </c>
       <c r="F72" s="15">
         <f>'3_SEMESTRE'!I13</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G72" s="44">
         <v>12</v>
@@ -10426,7 +10400,7 @@
       </c>
       <c r="F73" s="15">
         <f>'3_SEMESTRE'!K4</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G73" s="119">
         <f>'3_SEMESTRE'!K3</f>
@@ -10465,7 +10439,7 @@
       </c>
       <c r="F74" s="15">
         <f>'3_SEMESTRE'!K6</f>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G74" s="119">
         <f>'3_SEMESTRE'!K5</f>
@@ -10504,7 +10478,7 @@
       </c>
       <c r="F75" s="15">
         <f>'3_SEMESTRE'!K9</f>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G75" s="119">
         <f>'3_SEMESTRE'!K8</f>
@@ -10543,7 +10517,7 @@
       </c>
       <c r="F76" s="15">
         <f>'3_SEMESTRE'!K11</f>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G76" s="119">
         <f>'3_SEMESTRE'!K10</f>
@@ -10621,7 +10595,7 @@
       </c>
       <c r="F78" s="105">
         <f>'4_SEMESTRE'!C4</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G78" s="104">
         <f>'4_SEMESTRE'!C3</f>
@@ -10660,7 +10634,7 @@
       </c>
       <c r="F79" s="15">
         <f>'4_SEMESTRE'!C6</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G79" s="44">
         <f>'4_SEMESTRE'!C5</f>
@@ -10699,7 +10673,7 @@
       </c>
       <c r="F80" s="15">
         <f>'4_SEMESTRE'!C9</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G80" s="44">
         <f>'4_SEMESTRE'!C8</f>
@@ -10738,7 +10712,7 @@
       </c>
       <c r="F81" s="15">
         <f>'4_SEMESTRE'!C11</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G81" s="44">
         <f>'4_SEMESTRE'!C10</f>
@@ -10777,7 +10751,7 @@
       </c>
       <c r="F82" s="15">
         <f>'4_SEMESTRE'!C13</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G82" s="44">
         <f>'4_SEMESTRE'!C12</f>
@@ -10816,7 +10790,7 @@
       </c>
       <c r="F83" s="15">
         <f>'4_SEMESTRE'!E4</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G83" s="44">
         <f>'4_SEMESTRE'!E3</f>
@@ -10855,7 +10829,7 @@
       </c>
       <c r="F84" s="15">
         <f>'4_SEMESTRE'!E6</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G84" s="44">
         <f>'4_SEMESTRE'!E5</f>
@@ -10894,7 +10868,7 @@
       </c>
       <c r="F85" s="15">
         <f>'4_SEMESTRE'!E9</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G85" s="44">
         <f>'4_SEMESTRE'!E8</f>
@@ -10933,7 +10907,7 @@
       </c>
       <c r="F86" s="15">
         <f>'4_SEMESTRE'!E11</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G86" s="44">
         <f>'4_SEMESTRE'!E10</f>
@@ -10972,7 +10946,7 @@
       </c>
       <c r="F87" s="15">
         <f>'4_SEMESTRE'!E13</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G87" s="44">
         <f>'4_SEMESTRE'!E12</f>
@@ -11011,7 +10985,7 @@
       </c>
       <c r="F88" s="15">
         <f>'4_SEMESTRE'!G4</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G88" s="44">
         <f>'4_SEMESTRE'!G3</f>
@@ -11050,7 +11024,7 @@
       </c>
       <c r="F89" s="15">
         <f>'4_SEMESTRE'!G6</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G89" s="44">
         <f>'4_SEMESTRE'!G5</f>
@@ -11089,7 +11063,7 @@
       </c>
       <c r="F90" s="15">
         <f>'4_SEMESTRE'!G9</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G90" s="44">
         <f>'4_SEMESTRE'!G8</f>
@@ -11128,7 +11102,7 @@
       </c>
       <c r="F91" s="15">
         <f>'4_SEMESTRE'!G11</f>
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="G91" s="44">
         <f>'4_SEMESTRE'!G10</f>
@@ -11167,7 +11141,7 @@
       </c>
       <c r="F92" s="15">
         <f>'4_SEMESTRE'!G13</f>
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="G92" s="44">
         <f>'4_SEMESTRE'!G12</f>
@@ -11245,7 +11219,7 @@
       </c>
       <c r="F94" s="15">
         <f>'4_SEMESTRE'!I6</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G94" s="44">
         <f>'4_SEMESTRE'!I5</f>
@@ -11284,7 +11258,7 @@
       </c>
       <c r="F95" s="15">
         <f>'4_SEMESTRE'!I9</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G95" s="44">
         <f>'4_SEMESTRE'!I8</f>
@@ -11323,7 +11297,7 @@
       </c>
       <c r="F96" s="15">
         <f>'4_SEMESTRE'!I11</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G96" s="44">
         <f>'4_SEMESTRE'!I10</f>
@@ -11362,7 +11336,7 @@
       </c>
       <c r="F97" s="15">
         <f>'4_SEMESTRE'!I13</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G97" s="44">
         <f>'4_SEMESTRE'!I12</f>
@@ -11401,7 +11375,7 @@
       </c>
       <c r="F98" s="15">
         <f>'4_SEMESTRE'!K4</f>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G98" s="44">
         <f>'4_SEMESTRE'!K3</f>
@@ -11440,7 +11414,7 @@
       </c>
       <c r="F99" s="15">
         <f>'4_SEMESTRE'!K6</f>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G99" s="44">
         <f>'4_SEMESTRE'!K5</f>
@@ -11479,7 +11453,7 @@
       </c>
       <c r="F100" s="15">
         <f>'4_SEMESTRE'!K9</f>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G100" s="44">
         <f>'4_SEMESTRE'!K8</f>
@@ -11518,7 +11492,7 @@
       </c>
       <c r="F101" s="15">
         <f>'4_SEMESTRE'!K11</f>
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G101" s="44">
         <f>'4_SEMESTRE'!K10</f>
@@ -11557,7 +11531,7 @@
       </c>
       <c r="F102" s="81">
         <f>'4_SEMESTRE'!K13</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G102" s="116">
         <f>'4_SEMESTRE'!K12</f>
@@ -11596,7 +11570,7 @@
       </c>
       <c r="F103" s="105">
         <f>'5_SEMESTRE'!C4</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G103" s="104">
         <f>'5_SEMESTRE'!C3</f>
@@ -11635,7 +11609,7 @@
       </c>
       <c r="F104" s="15">
         <f>'5_SEMESTRE'!C6</f>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G104" s="44">
         <f>'5_SEMESTRE'!C5</f>
@@ -11674,7 +11648,7 @@
       </c>
       <c r="F105" s="15">
         <f>'5_SEMESTRE'!C9</f>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G105" s="44">
         <f>'5_SEMESTRE'!C8</f>
@@ -11713,7 +11687,7 @@
       </c>
       <c r="F106" s="15">
         <f>'5_SEMESTRE'!C11</f>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G106" s="44">
         <f>'5_SEMESTRE'!C10</f>
@@ -11752,7 +11726,7 @@
       </c>
       <c r="F107" s="15">
         <f>'5_SEMESTRE'!C13</f>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G107" s="44">
         <f>'5_SEMESTRE'!C12</f>
@@ -11791,7 +11765,7 @@
       </c>
       <c r="F108" s="15">
         <f>'5_SEMESTRE'!E4</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G108" s="44">
         <f>'5_SEMESTRE'!E3</f>
@@ -11830,7 +11804,7 @@
       </c>
       <c r="F109" s="15">
         <f>'5_SEMESTRE'!E6</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G109" s="44">
         <f>'5_SEMESTRE'!E5</f>
@@ -11869,7 +11843,7 @@
       </c>
       <c r="F110" s="15">
         <f>'5_SEMESTRE'!E9</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G110" s="44">
         <f>'5_SEMESTRE'!E8</f>
@@ -11908,7 +11882,7 @@
       </c>
       <c r="F111" s="15">
         <f>'5_SEMESTRE'!E11</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G111" s="44">
         <f>'5_SEMESTRE'!E10</f>
@@ -11947,7 +11921,7 @@
       </c>
       <c r="F112" s="15">
         <f>'5_SEMESTRE'!E13</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G112" s="44">
         <f>'5_SEMESTRE'!E12</f>
@@ -11986,7 +11960,7 @@
       </c>
       <c r="F113" s="15">
         <f>'5_SEMESTRE'!G4</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G113" s="44">
         <f>'5_SEMESTRE'!G3</f>
@@ -12025,7 +11999,7 @@
       </c>
       <c r="F114" s="15">
         <f>'5_SEMESTRE'!G6</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G114" s="44">
         <f>'5_SEMESTRE'!G5</f>
@@ -12064,7 +12038,7 @@
       </c>
       <c r="F115" s="15">
         <f>'5_SEMESTRE'!G9</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G115" s="44">
         <f>'5_SEMESTRE'!G8</f>
@@ -12103,7 +12077,7 @@
       </c>
       <c r="F116" s="15">
         <f>'5_SEMESTRE'!G11</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G116" s="44">
         <f>'5_SEMESTRE'!G10</f>
@@ -12142,7 +12116,7 @@
       </c>
       <c r="F117" s="15">
         <f>'5_SEMESTRE'!G13</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G117" s="44">
         <f>'5_SEMESTRE'!G12</f>
@@ -12181,7 +12155,7 @@
       </c>
       <c r="F118" s="15">
         <f>'5_SEMESTRE'!I4</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G118" s="44">
         <f>'5_SEMESTRE'!I3</f>
@@ -12220,7 +12194,7 @@
       </c>
       <c r="F119" s="15">
         <f>'5_SEMESTRE'!I6</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G119" s="44">
         <f>'5_SEMESTRE'!I5</f>
@@ -12259,7 +12233,7 @@
       </c>
       <c r="F120" s="15">
         <f>'5_SEMESTRE'!I9</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G120" s="44">
         <f>'5_SEMESTRE'!I8</f>
@@ -12298,7 +12272,7 @@
       </c>
       <c r="F121" s="15">
         <f>'5_SEMESTRE'!I11</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G121" s="44">
         <f>'5_SEMESTRE'!I10</f>
@@ -12337,7 +12311,7 @@
       </c>
       <c r="F122" s="15">
         <f>'5_SEMESTRE'!I13</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G122" s="44">
         <f>'5_SEMESTRE'!I12</f>
@@ -12376,7 +12350,7 @@
       </c>
       <c r="F123" s="15">
         <f>'5_SEMESTRE'!K4</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G123" s="44">
         <f>'5_SEMESTRE'!K3</f>
@@ -12415,7 +12389,7 @@
       </c>
       <c r="F124" s="15">
         <f>'5_SEMESTRE'!K6</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G124" s="44">
         <f>'5_SEMESTRE'!K5</f>
@@ -12454,7 +12428,7 @@
       </c>
       <c r="F125" s="15">
         <f>'5_SEMESTRE'!K9</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G125" s="44">
         <f>'5_SEMESTRE'!K8</f>
@@ -12493,7 +12467,7 @@
       </c>
       <c r="F126" s="15">
         <f>'5_SEMESTRE'!K11</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G126" s="44">
         <f>'5_SEMESTRE'!K10</f>
@@ -12571,7 +12545,7 @@
       </c>
       <c r="F128" s="96">
         <f>'6_SEMESTRE'!C4</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G128" s="122">
         <f>'6_SEMESTRE'!C3</f>
@@ -12610,7 +12584,7 @@
       </c>
       <c r="F129" s="50">
         <f>'6_SEMESTRE'!C6</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G129" s="49">
         <f>'6_SEMESTRE'!C5</f>
@@ -12649,7 +12623,7 @@
       </c>
       <c r="F130" s="50">
         <f>'6_SEMESTRE'!C9</f>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G130" s="49">
         <f>'6_SEMESTRE'!C8</f>
@@ -12688,7 +12662,7 @@
       </c>
       <c r="F131" s="50">
         <f>'6_SEMESTRE'!C11</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G131" s="49">
         <f>'6_SEMESTRE'!C10</f>
@@ -12727,7 +12701,7 @@
       </c>
       <c r="F132" s="50">
         <f>'6_SEMESTRE'!C13</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G132" s="49">
         <f>'6_SEMESTRE'!C12</f>
@@ -12766,7 +12740,7 @@
       </c>
       <c r="F133" s="50">
         <f>'6_SEMESTRE'!E4</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G133" s="49">
         <f>'6_SEMESTRE'!E3</f>
@@ -12805,7 +12779,7 @@
       </c>
       <c r="F134" s="50">
         <f>'6_SEMESTRE'!E6</f>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G134" s="49">
         <f>'6_SEMESTRE'!E5</f>
@@ -12844,7 +12818,7 @@
       </c>
       <c r="F135" s="50">
         <f>'6_SEMESTRE'!E9</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G135" s="49">
         <f>'6_SEMESTRE'!E8</f>
@@ -12883,7 +12857,7 @@
       </c>
       <c r="F136" s="50">
         <f>'6_SEMESTRE'!E11</f>
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G136" s="49">
         <f>'6_SEMESTRE'!E10</f>
@@ -12922,7 +12896,7 @@
       </c>
       <c r="F137" s="50">
         <f>'6_SEMESTRE'!E13</f>
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G137" s="49">
         <f>'6_SEMESTRE'!E12</f>
@@ -12961,7 +12935,7 @@
       </c>
       <c r="F138" s="55">
         <f>'6_SEMESTRE'!G4</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G138" s="48">
         <f>'6_SEMESTRE'!G3</f>
@@ -13000,7 +12974,7 @@
       </c>
       <c r="F139" s="55">
         <f>'6_SEMESTRE'!G6</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G139" s="48">
         <f>'6_SEMESTRE'!G5</f>
@@ -13039,7 +13013,7 @@
       </c>
       <c r="F140" s="55">
         <f>'6_SEMESTRE'!G9</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G140" s="48">
         <f>'6_SEMESTRE'!G8</f>
@@ -13078,7 +13052,7 @@
       </c>
       <c r="F141" s="55">
         <f>'6_SEMESTRE'!G11</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G141" s="48">
         <f>'6_SEMESTRE'!G10</f>
@@ -13117,7 +13091,7 @@
       </c>
       <c r="F142" s="55">
         <f>'6_SEMESTRE'!G13</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G142" s="48">
         <f>'6_SEMESTRE'!G12</f>
@@ -13156,7 +13130,7 @@
       </c>
       <c r="F143" s="50">
         <f>'6_SEMESTRE'!I4</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G143" s="49">
         <f>'6_SEMESTRE'!I3</f>
@@ -13195,7 +13169,7 @@
       </c>
       <c r="F144" s="50">
         <f>'6_SEMESTRE'!I6</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G144" s="49">
         <f>'6_SEMESTRE'!I5</f>
@@ -13234,7 +13208,7 @@
       </c>
       <c r="F145" s="50">
         <f>'6_SEMESTRE'!I9</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G145" s="49">
         <f>'6_SEMESTRE'!I8</f>
@@ -13273,7 +13247,7 @@
       </c>
       <c r="F146" s="50">
         <f>'6_SEMESTRE'!I11</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G146" s="49">
         <f>'6_SEMESTRE'!I10</f>
@@ -13312,7 +13286,7 @@
       </c>
       <c r="F147" s="50">
         <f>'6_SEMESTRE'!I13</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G147" s="49">
         <f>'6_SEMESTRE'!I12</f>
@@ -13351,7 +13325,7 @@
       </c>
       <c r="F148" s="55">
         <f>'6_SEMESTRE'!K4</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G148" s="48">
         <f>'6_SEMESTRE'!K3</f>
@@ -13390,7 +13364,7 @@
       </c>
       <c r="F149" s="55">
         <f>'6_SEMESTRE'!K6</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G149" s="48">
         <f>'6_SEMESTRE'!K5</f>
@@ -13429,7 +13403,7 @@
       </c>
       <c r="F150" s="55">
         <f>'6_SEMESTRE'!K9</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G150" s="48">
         <f>'6_SEMESTRE'!K8</f>
@@ -13468,7 +13442,7 @@
       </c>
       <c r="F151" s="55">
         <f>'6_SEMESTRE'!K11</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G151" s="48">
         <f>'6_SEMESTRE'!K10</f>

</xml_diff>